<commit_message>
use lower case except for the first character in papers' titles
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78A9AFD-F38A-424F-9F13-D95315EEDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CAF65E-133A-D44E-BF25-5C200EA2F4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -70,36 +70,6 @@
     <t>Van Hul</t>
   </si>
   <si>
-    <t xml:space="preserve">Impaired Adipose Tissue Development in Mice With Inactivation of Placental Growth Factor Function </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adipose Tissue Expression of Gelatinases in Mouse Models of Obesity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modulation of Adipose Tissue Expression of Murine Matrix Metalloproteinases and Their Tissue Inhibitors With Obesity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influence of PAI-1 on Adipose Tissue Growth and Metabolic Parameters in a Murine Model of Diet-Induced Obesity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modulation of Angiogenesis during Adipose Tissue Development in Murine Models of Obesity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutritionally Induced Obesity Is Attenuated in Transgenic Mice Overexpressing Plasminogen Activator Inhibitor-1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deficiency of tissue inhibitor of matrix metalloproteinase-1 (TIMP-1) impairs nutritionally induced obesity in mice </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enhanced nutritionally induced adipose tissue development in mice with stromelysin-1 gene inactivation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deficiency of plasminogen activator inhibitor-2 impairs nutritionally induced murine adipose tissue development </t>
-  </si>
-  <si>
-    <t>Role of thrombospondin-2 in Murine Adipose tissue Angiogenesis and Development</t>
-  </si>
-  <si>
     <t>Mesquita</t>
   </si>
   <si>
@@ -112,15 +82,6 @@
     <t>Koyama</t>
   </si>
   <si>
-    <t>Effects of Vascular-endothelial Protein tyrosine Phosphatase inhibition on Breast cancer Vasculature and Metastatic Progression</t>
-  </si>
-  <si>
-    <t>Tumor Blood Flow Differs between Mouse Strains: Consequences for Vasoresponse to Photodynamic Therapy</t>
-  </si>
-  <si>
-    <t>Interstitial Fluid Pressure and Capillary Diameter Distribution in Human Melanoma Xenografts</t>
-  </si>
-  <si>
     <t>Tumour blood vessel normalisation by prolyl hydroxylase inhibitor repaired sensitivity to chemotherapy in a tumour mouse model</t>
   </si>
   <si>
@@ -136,10 +97,6 @@
     <t>Stroma-derived but not tumor ADAMTS1 is a main driver of tumor growth and metastasis</t>
   </si>
   <si>
-    <t>FAK-heterozygous mice display enhanced tumour
-angiogenesis</t>
-  </si>
-  <si>
     <t>Endogenous ribosomal protein L29 (RPL29): a newly identified regulator of angiogenesis in mice</t>
   </si>
   <si>
@@ -179,31 +136,12 @@
     <t>Belligoli</t>
   </si>
   <si>
-    <t>Anatomy of the Mouse Retina. Capillary Basement Membrane Thickness</t>
-  </si>
-  <si>
-    <t>Electron Microscopy of Renal and Ocular Changes in Virus-Induced Diabetes Mellitus in Mice</t>
-  </si>
-  <si>
     <t>Age‐related ultrastructural changes of the basement membrane in the mouse blood‐brain barrier</t>
   </si>
   <si>
-    <t>Vascular Basement Membrane Thickness in Muscle of Spiny Mice and Activities of Glycolysis and Gluconeogenesis in the Liver of Animals with Spontaneous and Experimental Diabetes and of Untreated Human Diabetics</t>
-  </si>
-  <si>
-    <t>Ultrastructural Morphometry of Capillary Basement Membrane Thickness in Normal and Transgenic Diabetic Mice</t>
-  </si>
-  <si>
-    <t>Diabetic Kidney Disease in FVB/NJ Akita Mice: Temporal
-Pattern of Kidney Injury and Urinary Nephrin Excretion</t>
-  </si>
-  <si>
     <t>Glycosaminoglycans prevent morphological renal alterations and albuminuria in diabetic rats</t>
   </si>
   <si>
-    <t>Quantitative Estimation of Age-Related Thickening of Glomerular Basement Membrane in Normal Rats</t>
-  </si>
-  <si>
     <t>Blood glucose control and glomerular capillary basement membrane thickening in experimental diabetes</t>
   </si>
   <si>
@@ -325,6 +263,66 @@
   </si>
   <si>
     <t>Overexpression of VEGF189 in breast cancer cells induces apoptosis via NRP1 under stress conditions</t>
+  </si>
+  <si>
+    <t>Tumor blood flow differs between mouse strains: consequences for vasoresponse to photodynamic therapy</t>
+  </si>
+  <si>
+    <t>Effects of vascular-endothelial protein tyrosine phosphatase inhibition on breast cancer vasculature and metastatic progression</t>
+  </si>
+  <si>
+    <t>Interstitial fluid pressure and capillary diameter distribution in human melanoma xenografts</t>
+  </si>
+  <si>
+    <t>Anatomy of the mouse retina. capillary basement membrane thickness</t>
+  </si>
+  <si>
+    <t>Electron microscopy of renal and ocular changes in virus-induced diabetes mellitus in mice</t>
+  </si>
+  <si>
+    <t>Vascular basement membrane thickness in muscle of spiny mice and activities of glycolysis and gluconeogenesis in the liver of animals with spontaneous and experimental diabetes and of untreated human diabetics</t>
+  </si>
+  <si>
+    <t>Ultrastructural morphometry of capillary basement membrane thickness in normal and transgenic diabetic mice</t>
+  </si>
+  <si>
+    <t>FAK-heterozygous mice display enhanced tumour angiogenesis</t>
+  </si>
+  <si>
+    <t>Quantitative estimation of age-Related thickening of glomerular basement membrane in normal rats</t>
+  </si>
+  <si>
+    <t>Impaired adipose tissue development in mice with inactivation of placental growth factor function</t>
+  </si>
+  <si>
+    <t>Adipose tissue expression of gelatinases in mouse models of obesity</t>
+  </si>
+  <si>
+    <t>Modulation of adipose tissue expression of murine matrix metalloproteinases and their tissue inhibitors with obesity</t>
+  </si>
+  <si>
+    <t>Influence of PAI-1 on adipose tissue growth and metabolic parameters in a murine model of diet-induced obesity</t>
+  </si>
+  <si>
+    <t>Modulation of angiogenesis during adipose tissue development in murine models of obesity</t>
+  </si>
+  <si>
+    <t>Nutritionally induced obesity Is attenuated in transgenic mice overexpressing plasminogen activator inhibitor-1</t>
+  </si>
+  <si>
+    <t>Deficiency of tissue inhibitor of matrix metalloproteinase-1 (TIMP-1) impairs nutritionally induced obesity in mice</t>
+  </si>
+  <si>
+    <t>Enhanced nutritionally induced adipose tissue development in mice with stromelysin-1 gene inactivation</t>
+  </si>
+  <si>
+    <t>Diabetic kidney disease in FVB/NJ akita mice: temporal pattern of kidney injury and urinary nephrin excretion</t>
+  </si>
+  <si>
+    <t>Deficiency of plasminogen activator inhibitor‐2 impairs nutritionally induced murine adipose tissue development</t>
+  </si>
+  <si>
+    <t>Role of thrombospondin‐2 in murine adipose tissue angiogenesis and development</t>
   </si>
 </sst>
 </file>
@@ -704,7 +702,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C11"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,7 +729,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -742,7 +740,7 @@
         <v>2001</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -753,7 +751,7 @@
         <v>2002</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -764,7 +762,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -775,7 +773,7 @@
         <v>2005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -786,7 +784,7 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -797,7 +795,7 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -808,7 +806,7 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -819,7 +817,7 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -830,7 +828,7 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -843,7 +841,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,7 +868,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -881,7 +879,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -892,7 +890,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -903,7 +901,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -914,7 +912,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -925,7 +923,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -936,7 +934,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -948,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7CD81-0ECC-6140-89FA-3244ADAD567D}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,7 +974,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -987,7 +985,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -998,7 +996,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1009,7 +1007,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1020,7 +1018,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1031,7 +1029,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1042,7 +1040,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1076,46 +1074,46 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6">
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6">
         <v>2013</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6">
         <v>1999</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6">
         <v>2017</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1126,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,68 +1147,68 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6">
         <v>2013</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6">
         <v>1999</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6">
         <v>2016</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6">
         <v>2013</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6">
         <v>2013</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6">
         <v>2017</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1221,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,68 +1243,68 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3">
         <v>1986</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>1983</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3">
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3">
         <v>1970</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>2003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1317,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1340,68 +1338,68 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3">
         <v>1989</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3">
         <v>1993</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3">
         <v>1992</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3">
         <v>1978</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3">
         <v>1977</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1436,145 +1434,145 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6">
         <v>1994</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6">
         <v>2020</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6">
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6">
         <v>2002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6">
         <v>2012</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6">
         <v>2007</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B8" s="6">
         <v>1995</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6">
         <v>1999</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B10" s="6">
         <v>2005</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B11" s="6">
         <v>1998</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B12" s="6">
         <v>2001</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B13" s="6">
         <v>1999</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B14" s="6">
         <v>1992</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1611,101 +1609,101 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3">
         <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3">
         <v>1996</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3">
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3">
         <v>2002</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3">
         <v>2005</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B10" s="3">
         <v>2011</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit the papers' titles so that they are same as titles in CSV files
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CAF65E-133A-D44E-BF25-5C200EA2F4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D357382-EAED-3B41-A294-CFED1B5E1E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="4" activeTab="7" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>Characterization of receptor binding kinetics for vascular endothelial growth factor-A using SPR</t>
   </si>
   <si>
-    <t>Characterization of the vascular endothelial growth factor-receptor interaction and determination of the recombinant protein by an optical receptor sensor</t>
-  </si>
-  <si>
     <t>Binding and neutralization of vascular endothelial growth factor (VEGF) and related ligands by VEGF Trap, ranibizumab and bevacizumab</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>Vascular Endothelial Growth Factor Receptor-2 and Neuropilin-1 Form a Receptor Complex that is Responsible for the Differential Signaling Potency of VEGF165 and VEGF121</t>
   </si>
   <si>
-    <t>Characterization of vascular endothelial cell growth factor interactions with the kinase insert domain-containing receptor tyrosine kinase. A real time kinetic study</t>
-  </si>
-  <si>
     <t>Identification of the KDR tyrosine kinase as a receptor for vascular endothelial cell growth factor</t>
   </si>
   <si>
@@ -323,6 +317,12 @@
   </si>
   <si>
     <t>Role of thrombospondin‐2 in murine adipose tissue angiogenesis and development</t>
+  </si>
+  <si>
+    <t>Characterization of the vascular endothelial growth factor–receptor interaction and determination of the recombinant protein by an optical receptor sensor</t>
+  </si>
+  <si>
+    <t>Characterization of vascular endothelial cell growth factor interactions with the kinase insert domain-containing receptor tyrosine kinase: a real time kinetic study</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -740,7 +740,7 @@
         <v>2001</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2002</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>2005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -784,7 +784,7 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +868,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7CD81-0ECC-6140-89FA-3244ADAD567D}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -974,7 +974,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1080,7 @@
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>2013</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>1999</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1153,7 +1153,7 @@
         <v>2013</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>1999</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>2013</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>1986</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
         <v>1983</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>1970</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1293,7 +1293,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1304,7 +1304,7 @@
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1377,7 @@
         <v>1978</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1411,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1473,7 +1473,7 @@
         <v>2002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1484,7 +1484,7 @@
         <v>2012</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1506,7 +1506,7 @@
         <v>1995</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>1999</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1528,51 +1528,51 @@
         <v>2005</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="6">
         <v>1998</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="6">
         <v>2001</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="6">
         <v>1999</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6">
         <v>1992</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,57 +1609,57 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3">
         <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3">
         <v>1996</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1675,13 +1675,13 @@
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3">
         <v>2002</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1692,18 +1692,18 @@
         <v>2005</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3">
         <v>2011</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typo (`Creutzfelt` -> `Creutzfeldt`)
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D357382-EAED-3B41-A294-CFED1B5E1E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF66277C-B25C-584C-BB63-6555F3ED5D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="4" activeTab="7" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="4" activeTab="5" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Ceafalan</t>
   </si>
   <si>
-    <t>Creutzfelt</t>
-  </si>
-  <si>
     <t>Carlson</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Characterization of vascular endothelial cell growth factor interactions with the kinase insert domain-containing receptor tyrosine kinase: a real time kinetic study</t>
+  </si>
+  <si>
+    <t>Creutzfeldt</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -740,7 +740,7 @@
         <v>2001</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2002</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>2005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -784,7 +784,7 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +868,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +974,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1080,7 @@
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>2013</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>1999</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1153,7 +1153,7 @@
         <v>2013</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>1999</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>2013</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1220,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1249,7 +1249,7 @@
         <v>1986</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
         <v>1983</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1271,40 +1271,40 @@
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3">
         <v>1970</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3">
         <v>2003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1338,68 +1338,68 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3">
         <v>1989</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3">
         <v>1993</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3">
         <v>1992</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3">
         <v>1978</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3">
         <v>1977</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1411,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,145 +1434,145 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6">
         <v>1994</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6">
         <v>2020</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6">
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="6">
         <v>2002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6">
         <v>2012</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6">
         <v>2007</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="6">
         <v>1995</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="6">
         <v>1999</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="6">
         <v>2005</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="6">
         <v>1998</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6">
         <v>2001</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="6">
         <v>1999</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6">
         <v>1992</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,101 +1609,101 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3">
         <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
         <v>1996</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3">
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="3">
         <v>2002</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3">
         <v>2005</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3">
         <v>2011</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use lower case except for the first letter in title
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D20A11-4681-FA45-92F4-F86DB988CA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4F500-051D-8846-8974-39C146387000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" firstSheet="4" activeTab="6" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -289,9 +289,6 @@
     <t>Modulation of angiogenesis during adipose tissue development in murine models of obesity</t>
   </si>
   <si>
-    <t>Nutritionally induced obesity Is attenuated in transgenic mice overexpressing plasminogen activator inhibitor-1</t>
-  </si>
-  <si>
     <t>Deficiency of tissue inhibitor of matrix metalloproteinase-1 (TIMP-1) impairs nutritionally induced obesity in mice</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Quantitative estimation of age-related thickening of glomerular basement membrane in normal rats</t>
+  </si>
+  <si>
+    <t>Nutritionally induced obesity is attenuated in transgenic mice overexpressing plasminogen activator inhibitor-1</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,7 +784,7 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +841,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -890,7 +890,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7CD81-0ECC-6140-89FA-3244ADAD567D}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +996,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="3">
         <v>1970</v>
@@ -1304,7 +1304,7 @@
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1316,7 +1316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1377,7 +1377,7 @@
         <v>1978</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1473,7 +1473,7 @@
         <v>2002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1561,7 +1561,7 @@
         <v>1999</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1637,7 +1637,7 @@
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1648,7 +1648,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
edit the first author's name (`Ireland` -> `Fox`)
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4F500-051D-8846-8974-39C146387000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617AD3FC-8A27-1743-80FD-F54E13E8964E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" activeTab="2" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" firstSheet="2" activeTab="6" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>Yagihashi</t>
   </si>
   <si>
-    <t>Ireland</t>
-  </si>
-  <si>
     <t>Belligoli</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Nutritionally induced obesity is attenuated in transgenic mice overexpressing plasminogen activator inhibitor-1</t>
+  </si>
+  <si>
+    <t>Fox</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -740,7 +740,7 @@
         <v>2001</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>2002</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>2000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>2005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -784,7 +784,7 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -817,7 +817,7 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -828,7 +828,7 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +868,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -934,7 +934,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -946,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7CD81-0ECC-6140-89FA-3244ADAD567D}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -974,7 +974,7 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -985,7 +985,7 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1080,7 @@
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1091,7 +1091,7 @@
         <v>2013</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1102,7 +1102,7 @@
         <v>1999</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1153,7 +1153,7 @@
         <v>2013</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
         <v>1999</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>2013</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>1986</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1260,7 +1260,7 @@
         <v>1983</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1271,18 +1271,18 @@
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="3">
         <v>1970</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1293,7 +1293,7 @@
         <v>2003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1304,7 +1304,7 @@
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,7 +1344,7 @@
         <v>1989</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1355,7 +1355,7 @@
         <v>1993</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1366,7 +1366,7 @@
         <v>1992</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1377,29 +1377,29 @@
         <v>1978</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3">
         <v>1977</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1412,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,145 +1434,145 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6">
         <v>1994</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6">
         <v>2020</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6">
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6">
         <v>2002</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="6">
         <v>2012</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6">
         <v>2007</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="6">
         <v>1995</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6">
         <v>1999</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6">
         <v>2005</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6">
         <v>1998</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6">
         <v>2001</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6">
         <v>1999</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6">
         <v>1992</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1609,101 +1609,101 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3">
         <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3">
         <v>1996</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3">
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="3">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3">
         <v>2002</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3">
         <v>2005</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3">
         <v>2011</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add [Herve, 2008] and [Lu, 2023]
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4B7D6E-920A-2E49-ACAF-CB9C8B344D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760DCF13-20B6-AE43-9D6A-1F48DFAA1F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22900" firstSheet="2" activeTab="5" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" firstSheet="2" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="97">
   <si>
     <t>Title</t>
   </si>
@@ -323,6 +323,18 @@
   </si>
   <si>
     <t>Diabetic kidney disease in FVB/NJ Akita mice: temporal pattern of kidney injury and urinary nephrin excretion</t>
+  </si>
+  <si>
+    <t>Hervé</t>
+  </si>
+  <si>
+    <t>Overexpression of vascular endothelial growth factor 189 in breast cancer cells leads to delayed tumor uptake with dilated intratumoral vessels</t>
+  </si>
+  <si>
+    <t>Lu</t>
+  </si>
+  <si>
+    <t>A novel blood–brain barrier-penetrating and vascular-targeting chimeric peptide inhibits glioma angiogenesis</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1585,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,6 +1718,28 @@
         <v>65</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2008</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit list of papers read for meta-analysis and add column to show if Yunjeong read the paper or not
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5F67C9-704A-A847-A916-D07558C77708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC8188C-137B-D544-BCDE-7DCA66DFDC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" firstSheet="2" activeTab="6" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Kd_for_VEGFR1_and_VEGFR2" sheetId="7" r:id="rId8"/>
     <sheet name="Kd_for_NRP1" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="150">
   <si>
     <t>Title</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Tumour blood vessel normalisation by prolyl hydroxylase inhibitor repaired sensitivity to chemotherapy in a tumour mouse model</t>
   </si>
   <si>
-    <t>Fernandez</t>
-  </si>
-  <si>
     <t>Kostourou</t>
   </si>
   <si>
@@ -341,6 +338,164 @@
   </si>
   <si>
     <t>Ocular complications in the old and glucose-intolerant genetically obese (fa/fa) rat</t>
+  </si>
+  <si>
+    <t>Colotti</t>
+  </si>
+  <si>
+    <t>Geretti</t>
+  </si>
+  <si>
+    <t>Guerrin</t>
+  </si>
+  <si>
+    <t>Sarabipour</t>
+  </si>
+  <si>
+    <t>Shibuya</t>
+  </si>
+  <si>
+    <t>Tillo</t>
+  </si>
+  <si>
+    <t>Bloodworth</t>
+  </si>
+  <si>
+    <t>Fu</t>
+  </si>
+  <si>
+    <t>Leclech</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>Saito</t>
+  </si>
+  <si>
+    <t>Thomsen</t>
+  </si>
+  <si>
+    <t>Velic</t>
+  </si>
+  <si>
+    <t>Welt</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Cherian</t>
+  </si>
+  <si>
+    <t>Lang</t>
+  </si>
+  <si>
+    <t>Sletta</t>
+  </si>
+  <si>
+    <t>Cai</t>
+  </si>
+  <si>
+    <t>Three-dimensional quantification of capillary networks in healthy and cancerous tissues of two mice</t>
+  </si>
+  <si>
+    <t>Oxygen-dependent regulation of tumor growth and metastasis in human breast cancer xenografts</t>
+  </si>
+  <si>
+    <t>PET of vascular endothelial growth factor receptor expression</t>
+  </si>
+  <si>
+    <t>Transendothelial insulin transport is impaired in skeletal muscle capillaries of obese male mice</t>
+  </si>
+  <si>
+    <t>Variations in capillary basement membrane width produced by aging and diabetes mellitus</t>
+  </si>
+  <si>
+    <t>Insulin’s actions on vascular tissues: Physiological effects and pathophysiological contributions to vascular complications of diabetes</t>
+  </si>
+  <si>
+    <t>The basement membrane as a structured surface – role in vascular health and disease</t>
+  </si>
+  <si>
+    <t>Retinal capillary basement membrane thickening: Role in the pathogenesis of diabetic retinopathy</t>
+  </si>
+  <si>
+    <t>Vascular basement membrane thickening in diabetic retinopathy</t>
+  </si>
+  <si>
+    <t>Alteration in haemodynamics and pathological changes in the cardiovascular system during the development of Type 2 diabetes mellitus in OLETF rats</t>
+  </si>
+  <si>
+    <t>The vascular basement membrane in the healthy and pathological brain</t>
+  </si>
+  <si>
+    <t>Diabetic basement membrane thickening does not occur in myocardial capillaries of transgenic mice when metallothionein is overexpressed in cardiac myocytes</t>
+  </si>
+  <si>
+    <t>Protective effects of Ginkgo biloba extract EGb 761 on the myocardium of experimentally diabetic rats</t>
+  </si>
+  <si>
+    <t>Tight glycemic control regulates fibronectin expression and basement membrane thickening in retinal and glomerular capillaries of diabetic rats</t>
+  </si>
+  <si>
+    <t>Selected</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Neuropilin-1 is required for endothelial cell adhesion to soluble vascular endothelial growth factor receptor 1</t>
+  </si>
+  <si>
+    <t>Site-directed Mutagenesis in the B-Neuropilin-2 Domain Selectively Enhances Its Affinity to VEGF165, but Not to
+Semaphorin 3F</t>
+  </si>
+  <si>
+    <t>VasculotropinNascular EndothelialGrowth Factor Is an Autocrine Growth Factor for Human Retinal Pigment Epithelial Cells Cultured In Vitro</t>
+  </si>
+  <si>
+    <t>Papo</t>
+  </si>
+  <si>
+    <t>Antagonistic VEGF variants engineered to simultaneously bind to and inhibit
+VEGFR2 and αvβ3 integrin</t>
+  </si>
+  <si>
+    <t>VEGF-A121a binding to Neuropilins – A concept revisited</t>
+  </si>
+  <si>
+    <t>Nucleotide sequence and expression of a novel human receptor-type tyrosine kinase gene (fit) closely related to the fms family</t>
+  </si>
+  <si>
+    <t>VEGF189 binds NRP1 and is sufficient for VEGF/NRP1-dependent neuronal patterning in the developing brain</t>
+  </si>
+  <si>
+    <t>VEGF165 Mediates Formation of Complexes Containing VEGFR-2 and Neuropilin-1 That Enhance VEGF165-Receptor Binding</t>
+  </si>
+  <si>
+    <t>Mamluk</t>
+  </si>
+  <si>
+    <t>Neuropilin-1 Binds Vascular Endothelial Growth Factor 165, Placenta Growth Factor-2, and Heparin via Its b1b2 Domain</t>
+  </si>
+  <si>
+    <t>Fraselle-Jacobs</t>
+  </si>
+  <si>
+    <t>Effect of aging on the morphology of epididymal adipose tissue in the rat</t>
+  </si>
+  <si>
+    <t>Begieneman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The basement membrane of intramyocardial capillaries is thickened in patients with acute myocardial infarction </t>
+  </si>
+  <si>
+    <t>Fernandez-Rodriguez</t>
   </si>
 </sst>
 </file>
@@ -383,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -402,6 +557,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91159889-8DB1-3746-A905-7DDAE9ADC690}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +893,7 @@
     <col min="3" max="3" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -738,8 +903,11 @@
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -747,10 +915,13 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -758,10 +929,13 @@
         <v>2001</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -769,10 +943,13 @@
         <v>2002</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -780,10 +957,13 @@
         <v>2000</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -791,10 +971,13 @@
         <v>2005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -802,10 +985,13 @@
         <v>2003</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
@@ -813,10 +999,13 @@
         <v>2003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -824,10 +1013,13 @@
         <v>2003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
@@ -835,10 +1027,13 @@
         <v>2007</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -846,7 +1041,10 @@
         <v>2012</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -856,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738AA7C5-4037-8340-B7D1-2CDE07BD0EFC}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D8" sqref="D1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,7 +1065,7 @@
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -877,8 +1075,11 @@
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -886,10 +1087,13 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -897,10 +1101,13 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -908,10 +1115,13 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -919,10 +1129,13 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -930,10 +1143,13 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -941,10 +1157,13 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -952,7 +1171,10 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -962,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7CD81-0ECC-6140-89FA-3244ADAD567D}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,7 +1195,7 @@
     <col min="3" max="3" width="68.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -983,8 +1205,11 @@
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -992,10 +1217,13 @@
         <v>2006</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1003,10 +1231,13 @@
         <v>2005</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1014,10 +1245,13 @@
         <v>2003</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1025,10 +1259,13 @@
         <v>2003</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1036,10 +1273,13 @@
         <v>2003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1047,10 +1287,13 @@
         <v>2007</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1301,10 @@
         <v>2012</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1068,10 +1314,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658AB769-96F6-4F4E-AFE9-5D8CEE084699}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,7 +1325,7 @@
     <col min="3" max="3" width="57" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1089,8 +1335,11 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1098,10 +1347,13 @@
         <v>2012</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -1109,10 +1361,13 @@
         <v>2013</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1120,10 +1375,13 @@
         <v>1999</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1132,6 +1390,51 @@
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2017</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1141,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A43CD9-1228-D34B-A13B-159119F891BF}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,7 +1455,7 @@
     <col min="3" max="3" width="76.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1162,8 +1465,11 @@
       <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1171,10 +1477,13 @@
         <v>2013</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1182,43 +1491,55 @@
         <v>1999</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="B4" s="6">
         <v>2016</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6">
         <v>2013</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6">
         <v>2013</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -1227,6 +1548,37 @@
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2006</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2017</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1236,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1600,7 @@
     <col min="3" max="3" width="58.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1258,71 +1610,120 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3">
         <v>1986</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3">
         <v>1983</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3">
         <v>2019</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3">
         <v>1970</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3">
         <v>2003</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3">
         <v>2012</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2013</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1332,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,92 +1744,270 @@
     <col min="3" max="3" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1989</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3">
-        <v>1989</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="8">
+        <v>1993</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3">
-        <v>1993</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="8">
+        <v>1992</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3">
-        <v>1992</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="8">
+        <v>1978</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1977</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="D6" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3">
-        <v>1978</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1977</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="8">
+        <v>2019</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2019</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="D7" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1990</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="3">
-        <v>1990</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
+      <c r="D8" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1970</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2010</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2003</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2017</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1999</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2009</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1987</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2008</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1438,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,162 +2029,313 @@
     <col min="3" max="3" width="81.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="D1" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1994</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6">
-        <v>1994</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="7">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="D3" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="6">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="7">
+        <v>2002</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2007</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1995</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2005</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1998</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1999</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1992</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="7">
         <v>2019</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="6">
-        <v>2002</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2012</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="C14" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="7">
         <v>2007</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="C15" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="7">
         <v>1995</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1999</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2005</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1998</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="6">
-        <v>2001</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1999</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1992</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="C16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2011</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1990</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2015</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="3"/>
+      <c r="B21" s="3">
+        <v>1996</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2023</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1614,10 +2344,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1625,7 +2355,7 @@
     <col min="3" max="3" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1635,126 +2365,190 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3">
         <v>2001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3">
         <v>1996</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="3">
         <v>1998</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3">
         <v>2007</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="3">
         <v>2002</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>2005</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3">
         <v>2011</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="3">
         <v>2008</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="B12" s="3">
         <v>2023</v>
       </c>
-      <c r="C12" t="s">
-        <v>96</v>
+      <c r="C12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2002</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2002</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copy and paste title from Google Scholar and delete (Fu, 2020) from CBM thickness paper list
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC8188C-137B-D544-BCDE-7DCA66DFDC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2599E8-ECB8-B14D-B0E7-C4B3F78CDF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22900" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="0" yWindow="11960" windowWidth="44800" windowHeight="11460" firstSheet="2" activeTab="7" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="148">
   <si>
     <t>Title</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Bloodworth</t>
   </si>
   <si>
-    <t>Fu</t>
-  </si>
-  <si>
     <t>Leclech</t>
   </si>
   <si>
@@ -412,9 +409,6 @@
     <t>Variations in capillary basement membrane width produced by aging and diabetes mellitus</t>
   </si>
   <si>
-    <t>Insulin’s actions on vascular tissues: Physiological effects and pathophysiological contributions to vascular complications of diabetes</t>
-  </si>
-  <si>
     <t>The basement membrane as a structured surface – role in vascular health and disease</t>
   </si>
   <si>
@@ -431,9 +425,6 @@
   </si>
   <si>
     <t>Diabetic basement membrane thickening does not occur in myocardial capillaries of transgenic mice when metallothionein is overexpressed in cardiac myocytes</t>
-  </si>
-  <si>
-    <t>Protective effects of Ginkgo biloba extract EGb 761 on the myocardium of experimentally diabetic rats</t>
   </si>
   <si>
     <t>Tight glycemic control regulates fibronectin expression and basement membrane thickening in retinal and glomerular capillaries of diabetic rats</t>
@@ -496,6 +487,9 @@
   </si>
   <si>
     <t>Fernandez-Rodriguez</t>
+  </si>
+  <si>
+    <t>Protective effects of Ginkgo biloba extract EGb 761 on the myocardium of experimentally diabetic rats: II. Ultrastructural and immunohistochemical investigation on microvessels and interstitium</t>
   </si>
 </sst>
 </file>
@@ -538,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -557,16 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91159889-8DB1-3746-A905-7DDAE9ADC690}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D9"/>
     </sheetView>
   </sheetViews>
@@ -904,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -918,7 +902,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -932,7 +916,7 @@
         <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -946,7 +930,7 @@
         <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -960,7 +944,7 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -974,7 +958,7 @@
         <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -988,7 +972,7 @@
         <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1002,7 +986,7 @@
         <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1016,7 +1000,7 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1030,7 +1014,7 @@
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1044,7 +1028,7 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1090,7 +1074,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1104,7 +1088,7 @@
         <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1118,7 +1102,7 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1132,7 +1116,7 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1146,7 +1130,7 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1160,7 +1144,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1174,7 +1158,7 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1220,7 +1204,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1234,7 +1218,7 @@
         <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1248,7 +1232,7 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1262,7 +1246,7 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1276,7 +1260,7 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1290,7 +1274,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1304,7 +1288,7 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1350,7 +1334,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1364,7 +1348,7 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1378,7 +1362,7 @@
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1392,40 +1376,40 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="6">
         <v>2012</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="6">
         <v>2017</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B8" s="6">
         <v>2016</v>
@@ -1434,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1466,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1480,7 +1464,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1494,12 +1478,12 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B4" s="6">
         <v>2016</v>
@@ -1508,7 +1492,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1522,7 +1506,7 @@
         <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1536,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1550,35 +1534,35 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="6">
         <v>2006</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="6">
         <v>2017</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1625,7 +1609,7 @@
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1639,7 +1623,7 @@
         <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1653,7 +1637,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1667,7 +1651,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1681,7 +1665,7 @@
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1695,35 +1679,35 @@
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="3">
         <v>2020</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="3">
         <v>2013</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1733,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1745,269 +1729,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>131</v>
+      <c r="D1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="3">
         <v>1989</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>132</v>
+      <c r="D2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="3">
         <v>1993</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>132</v>
+      <c r="D3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="3">
         <v>1992</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>132</v>
+      <c r="D4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="3">
         <v>1978</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>132</v>
+      <c r="D5" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>1977</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>132</v>
+      <c r="D6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <v>2019</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>133</v>
+      <c r="D7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>1990</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>132</v>
+      <c r="D8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="3">
         <v>1970</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="8">
-        <v>2020</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2010</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="8">
-        <v>2020</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="8">
-        <v>2010</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="B13" s="3">
+        <v>2003</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="8">
-        <v>2021</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="8">
-        <v>2003</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="8">
-        <v>2017</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1999</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2009</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1999</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="8">
-        <v>2009</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>132</v>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1987</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2008</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="8">
-        <v>1987</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="8">
-        <v>2008</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>132</v>
+      <c r="D18" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2019,7 +1989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
@@ -2030,283 +2000,283 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1994</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2002</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2012</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2007</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1995</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1999</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2005</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1998</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1999</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1992</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1994</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2007</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="7">
-        <v>2020</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="7">
-        <v>2019</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1995</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="7">
-        <v>2002</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="7">
-        <v>2012</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="7">
-        <v>2007</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1995</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1999</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="7">
-        <v>2005</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1998</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1999</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1992</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="7">
-        <v>2019</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="D16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="7">
-        <v>2007</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B17" s="6">
+        <v>2011</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1995</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="D17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2018</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="D18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1990</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="7">
-        <v>2011</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2015</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2018</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="7">
-        <v>1990</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="7">
-        <v>2015</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>133</v>
+      <c r="D20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2320,7 +2290,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2334,7 +2304,7 @@
         <v>95</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2380,7 +2350,7 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2394,7 +2364,7 @@
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2408,7 +2378,7 @@
         <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2422,7 +2392,7 @@
         <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2436,7 +2406,7 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2450,7 +2420,7 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2464,7 +2434,7 @@
         <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2478,7 +2448,7 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2492,7 +2462,7 @@
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2506,7 +2476,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2520,7 +2490,7 @@
         <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2531,24 +2501,24 @@
         <v>2002</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B14" s="3">
         <v>2002</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copy and paste title from Google Scholar
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2599E8-ECB8-B14D-B0E7-C4B3F78CDF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4670C99A-2F4B-1C4D-A61A-2E6FD859CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11960" windowWidth="44800" windowHeight="11460" firstSheet="2" activeTab="7" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="0" yWindow="11960" windowWidth="44800" windowHeight="11460" firstSheet="2" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -409,9 +409,6 @@
     <t>Variations in capillary basement membrane width produced by aging and diabetes mellitus</t>
   </si>
   <si>
-    <t>The basement membrane as a structured surface – role in vascular health and disease</t>
-  </si>
-  <si>
     <t>Retinal capillary basement membrane thickening: Role in the pathogenesis of diabetic retinopathy</t>
   </si>
   <si>
@@ -439,41 +436,15 @@
     <t>No</t>
   </si>
   <si>
-    <t>Neuropilin-1 is required for endothelial cell adhesion to soluble vascular endothelial growth factor receptor 1</t>
-  </si>
-  <si>
-    <t>Site-directed Mutagenesis in the B-Neuropilin-2 Domain Selectively Enhances Its Affinity to VEGF165, but Not to
-Semaphorin 3F</t>
-  </si>
-  <si>
-    <t>VasculotropinNascular EndothelialGrowth Factor Is an Autocrine Growth Factor for Human Retinal Pigment Epithelial Cells Cultured In Vitro</t>
-  </si>
-  <si>
     <t>Papo</t>
   </si>
   <si>
-    <t>Antagonistic VEGF variants engineered to simultaneously bind to and inhibit
-VEGFR2 and αvβ3 integrin</t>
-  </si>
-  <si>
-    <t>VEGF-A121a binding to Neuropilins – A concept revisited</t>
-  </si>
-  <si>
-    <t>Nucleotide sequence and expression of a novel human receptor-type tyrosine kinase gene (fit) closely related to the fms family</t>
-  </si>
-  <si>
     <t>VEGF189 binds NRP1 and is sufficient for VEGF/NRP1-dependent neuronal patterning in the developing brain</t>
   </si>
   <si>
-    <t>VEGF165 Mediates Formation of Complexes Containing VEGFR-2 and Neuropilin-1 That Enhance VEGF165-Receptor Binding</t>
-  </si>
-  <si>
     <t>Mamluk</t>
   </si>
   <si>
-    <t>Neuropilin-1 Binds Vascular Endothelial Growth Factor 165, Placenta Growth Factor-2, and Heparin via Its b1b2 Domain</t>
-  </si>
-  <si>
     <t>Fraselle-Jacobs</t>
   </si>
   <si>
@@ -483,13 +454,40 @@
     <t>Begieneman</t>
   </si>
   <si>
-    <t xml:space="preserve">The basement membrane of intramyocardial capillaries is thickened in patients with acute myocardial infarction </t>
-  </si>
-  <si>
     <t>Fernandez-Rodriguez</t>
   </si>
   <si>
     <t>Protective effects of Ginkgo biloba extract EGb 761 on the myocardium of experimentally diabetic rats: II. Ultrastructural and immunohistochemical investigation on microvessels and interstitium</t>
+  </si>
+  <si>
+    <t>The basement membrane of intramyocardial capillaries is thickened in patients with acute myocardial infarction</t>
+  </si>
+  <si>
+    <t>The basement membrane as a structured surface–role in vascular health and disease</t>
+  </si>
+  <si>
+    <t>Site-directed mutagenesis in the B-neuropilin-2 domain selectively enhances its affinity to VEGF165, but not to semaphorin 3F</t>
+  </si>
+  <si>
+    <t>Vasculotropin/Vascular endothelial growth factor is an autocrine growth factor for human retinal pigment epithelial cells cultued in vitro</t>
+  </si>
+  <si>
+    <t>Antagonistic VEGF variants engineered to simultaneously bind to and inhibit VEGFR2 and α v β 3 integrin</t>
+  </si>
+  <si>
+    <t>VEGF-A121a binding to Neuropilins–A concept revisited</t>
+  </si>
+  <si>
+    <t>Neuropilin-1 binds vascular endothelial growth factor 165, placenta growth factor-2, and heparin via its b1b2 domain</t>
+  </si>
+  <si>
+    <t>VEGF165 mediates formation of complexes containing VEGFR‐2 and neuropilin‐1 that enhance VEGF165‐receptor binding</t>
+  </si>
+  <si>
+    <t>Nucleotide sequence and expression of a novel human receptor-type tyrosine kinase gene (flt) closely related to the fms family.</t>
+  </si>
+  <si>
+    <t>Neuropilin‐1 is required for endothelial cell adhesion to soluble vascular endothelial growth factor receptor 1</t>
   </si>
 </sst>
 </file>
@@ -888,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -902,7 +900,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -916,7 +914,7 @@
         <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -930,7 +928,7 @@
         <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -944,7 +942,7 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -958,7 +956,7 @@
         <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -972,7 +970,7 @@
         <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -986,7 +984,7 @@
         <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1000,7 +998,7 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1014,7 +1012,7 @@
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1028,7 +1026,7 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1060,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1074,7 +1072,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1088,7 +1086,7 @@
         <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1102,7 +1100,7 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1116,7 +1114,7 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1130,7 +1128,7 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1144,7 +1142,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1158,7 +1156,7 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1204,7 +1202,7 @@
         <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1218,7 +1216,7 @@
         <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1232,7 +1230,7 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1246,7 +1244,7 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1260,7 +1258,7 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1274,7 +1272,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1288,7 +1286,7 @@
         <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1334,7 +1332,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1348,7 +1346,7 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1362,7 +1360,7 @@
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1376,7 +1374,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1390,7 +1388,7 @@
         <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1404,12 +1402,12 @@
         <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B8" s="6">
         <v>2016</v>
@@ -1418,7 +1416,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1431,7 +1429,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1464,7 +1462,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1478,12 +1476,12 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B4" s="6">
         <v>2016</v>
@@ -1492,7 +1490,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1506,7 +1504,7 @@
         <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1520,7 +1518,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1534,7 +1532,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1548,7 +1546,7 @@
         <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1562,7 +1560,7 @@
         <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1595,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1609,7 +1607,7 @@
         <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1623,7 +1621,7 @@
         <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1637,7 +1635,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -1651,7 +1649,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1665,7 +1663,7 @@
         <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1679,7 +1677,7 @@
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1693,7 +1691,7 @@
         <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1704,10 +1702,10 @@
         <v>2013</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1719,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1739,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1753,7 +1751,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1767,7 +1765,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1781,7 +1779,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1795,7 +1793,7 @@
         <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1809,7 +1807,7 @@
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,7 +1821,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1837,7 +1835,7 @@
         <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1851,7 +1849,7 @@
         <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1862,10 +1860,10 @@
         <v>2020</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1876,10 +1874,10 @@
         <v>2010</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1890,10 +1888,10 @@
         <v>2021</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1904,10 +1902,10 @@
         <v>2003</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1918,10 +1916,10 @@
         <v>2017</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1932,10 +1930,10 @@
         <v>1999</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1946,38 +1944,38 @@
         <v>2009</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B17" s="3">
         <v>1987</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B18" s="3">
         <v>2008</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1987,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2024,7 +2022,7 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2038,7 +2036,7 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2052,7 +2050,7 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2066,7 +2064,7 @@
         <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2080,7 +2078,7 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2094,7 +2092,7 @@
         <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2108,7 +2106,7 @@
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2122,7 +2120,7 @@
         <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2136,7 +2134,7 @@
         <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2150,7 +2148,7 @@
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2164,7 +2162,7 @@
         <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2178,133 +2176,105 @@
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B14" s="6">
-        <v>2019</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>131</v>
+        <v>1995</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="D14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="B15" s="6">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="6">
-        <v>1995</v>
+        <v>2018</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1990</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>137</v>
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1996</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="6">
-        <v>2015</v>
+      <c r="A20" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2023</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1996</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2023</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2314,10 +2284,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2336,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2350,7 +2320,7 @@
         <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2364,7 +2334,7 @@
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2378,7 +2348,7 @@
         <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2392,7 +2362,7 @@
         <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2406,7 +2376,7 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2420,7 +2390,7 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2434,7 +2404,7 @@
         <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2448,7 +2418,7 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2462,7 +2432,7 @@
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2476,7 +2446,7 @@
         <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2490,7 +2460,7 @@
         <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2501,24 +2471,52 @@
         <v>2002</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B14" s="3">
         <v>2002</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2019</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2007</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add list of papers I read recently
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4670C99A-2F4B-1C4D-A61A-2E6FD859CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D810837B-EA3B-E143-8127-4927613AAF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11960" windowWidth="44800" windowHeight="11460" firstSheet="2" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="183">
   <si>
     <t>Title</t>
   </si>
@@ -488,13 +488,118 @@
   </si>
   <si>
     <t>Neuropilin‐1 is required for endothelial cell adhesion to soluble vascular endothelial growth factor receptor 1</t>
+  </si>
+  <si>
+    <t>Hawkes</t>
+  </si>
+  <si>
+    <t>Regional differences in the morphological and functional effects of aging on cerebral basement membranes and perivascular drainage of amyloid-β from the mouse brain</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t>Robison</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Zheng</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Downregulation of fibronectin overexpression reduces basement membrane thickening and vascular lesions in retinas of galactose-fed rats</t>
+  </si>
+  <si>
+    <t>Ultrastructural alterations in capillaries of the diabetic hypertensive rat retina: protective effects of ACE inhibition</t>
+  </si>
+  <si>
+    <t>Chakrabarti</t>
+  </si>
+  <si>
+    <t>McCaleb</t>
+  </si>
+  <si>
+    <t>Clements</t>
+  </si>
+  <si>
+    <t>Sima</t>
+  </si>
+  <si>
+    <t>Kern</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>Effect of aldose reductase inhibition and insulin treatment on retinal capillary basement membrane thickening in BB rats</t>
+  </si>
+  <si>
+    <t>Intervention with the aldose reductase inhibitor, tolrestat, in renal and retinal lesions of streptozotocin-diabetic rats</t>
+  </si>
+  <si>
+    <t>Prevention of basement membrane thickening in retinal capillaries by a novel inhibitor of aldose reductase, tolrestat</t>
+  </si>
+  <si>
+    <t>Anti-glycated albumin therapy ameliorates early retinal microvascular pathology in db/db mice</t>
+  </si>
+  <si>
+    <t>Pancreatic islet allograft prevents basement membrane thickening in the diabetic rat retina</t>
+  </si>
+  <si>
+    <t>Comparison of retinal lesions in alloxan-diabetic rats and galactose-fed rats</t>
+  </si>
+  <si>
+    <t>Anionic sites in diabetic basement membranes and their possible role in diffusion barrier abnormalities in the BB-rat</t>
+  </si>
+  <si>
+    <t>A long-term siRNA strategy regulates fibronectin overexpression and improves vascular lesions in retinas of diabetic rats</t>
+  </si>
+  <si>
+    <t>Increases in collagen type IV and laminin in galactose-induced retinal capillary basement membrane thickening—prevention by an aldose reductase inhibitor</t>
+  </si>
+  <si>
+    <t>Effects of angiotensin-converting enzyme inhibitors and β-adrenergic blockers on retinal vascular endothelial growth factor expression in rat diabetic retinopathy</t>
+  </si>
+  <si>
+    <t>Galactose-induced retinal capillary basement membrane thickening: prevention by Sorbinil.</t>
+  </si>
+  <si>
+    <t>RCapillaries: Basement Membrane Thickening by Galactosemia Prevented with Aldose Reductase Inhibitor</t>
+  </si>
+  <si>
+    <t>Endothelin receptor blockade prevents augmented extracellular matrix component mRNA expression and capillary basement membrane thickening in the retina of diabetic and galactose-fed rats.</t>
+  </si>
+  <si>
+    <t>Fenofibrate ameliorates oxidative stress-induced retinal microvascular dysfunction in diabetic rats</t>
+  </si>
+  <si>
+    <t>Tessler</t>
+  </si>
+  <si>
+    <t>Heparin modulates the interaction of VEGF165 with soluble and cell associated flk-1 receptors.</t>
+  </si>
+  <si>
+    <t>Gluzman-Poltorak</t>
+  </si>
+  <si>
+    <t>Neuropilin-2 and neuropilin-1 are receptors for the 165-amino acid form of vascular endothelial growth factor (VEGF) and of placenta growth factor-2, but only neuropilin-2 functions as a receptor for the 145-amino acid form of VEGF</t>
+  </si>
+  <si>
+    <t>von Wronski</t>
+  </si>
+  <si>
+    <t>Tuftsin binds neuropilin-1 through a sequence similar to that encoded by exon 8 of vascular endothelial growth factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -508,6 +613,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -530,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -550,6 +661,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,9 +687,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -608,7 +727,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -714,7 +833,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -856,7 +975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1570,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1708,6 +1827,20 @@
         <v>128</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2013</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1715,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1727,254 +1860,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>1989</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>1993</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>1992</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>1978</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="7">
         <v>1977</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <v>2019</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>1990</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="7">
         <v>1970</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="7">
         <v>2020</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="7">
         <v>2010</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="7">
         <v>2021</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="7">
         <v>2003</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="7">
         <v>2017</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="7">
         <v>1999</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="7">
         <v>2009</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="7">
         <v>1987</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="7">
         <v>2008</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="7">
+        <v>1990</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1983</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2003</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2007</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2004</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1983</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1989</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="7">
+        <v>1991</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1986</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1998</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1988</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1994</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1991</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2011</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2018</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1985,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2277,6 +2634,20 @@
         <v>128</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1994</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2284,10 +2655,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2519,6 +2890,34 @@
         <v>129</v>
       </c>
     </row>
+    <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2006</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
match title with Google Scholar
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D810837B-EA3B-E143-8127-4927613AAF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841BC58-AB3E-C642-BA42-46C653EAA050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="8" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="5" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -493,9 +493,6 @@
     <t>Hawkes</t>
   </si>
   <si>
-    <t>Regional differences in the morphological and functional effects of aging on cerebral basement membranes and perivascular drainage of amyloid-β from the mouse brain</t>
-  </si>
-  <si>
     <t>Das</t>
   </si>
   <si>
@@ -593,6 +590,9 @@
   </si>
   <si>
     <t>Tuftsin binds neuropilin-1 through a sequence similar to that encoded by exon 8 of vascular endothelial growth factor</t>
+  </si>
+  <si>
+    <t>Regional differences in the morphological and functional effects of aging on cerebral basement membranes and perivascular drainage of amyloid‐β from the mouse brain</t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -660,13 +660,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1691,7 +1684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1835,7 +1828,7 @@
         <v>2013</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="D10" t="s">
         <v>128</v>
@@ -1860,478 +1853,478 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="3">
         <v>1989</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>1993</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>1992</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="3">
         <v>1978</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="3">
         <v>1977</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="3">
         <v>2019</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="3">
         <v>1990</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="3">
         <v>1970</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="3">
         <v>2020</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="3">
         <v>2010</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="3">
         <v>2021</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="3">
         <v>2003</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="3">
         <v>2017</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="3">
         <v>1999</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="3">
         <v>2009</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="3">
         <v>1987</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
+      <c r="A18" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="3">
         <v>2008</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1990</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B19" s="7">
-        <v>1990</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B20" s="3">
+        <v>1983</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2003</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B22" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2007</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="7">
+      <c r="D23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2004</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="3">
         <v>1983</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="C25" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1989</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1991</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1986</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1998</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1988</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1994</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1991</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="7">
-        <v>2003</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B22" s="7">
-        <v>2000</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B33" s="3">
+        <v>2011</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2018</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="7">
-        <v>2007</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="7">
-        <v>2004</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="7">
-        <v>1983</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1989</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B27" s="7">
-        <v>1991</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1986</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B29" s="7">
-        <v>1998</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="B30" s="7">
-        <v>1988</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1994</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1991</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="7">
-        <v>2011</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B34" s="7">
-        <v>2018</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2636,13 +2629,13 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B21" s="6">
         <v>1994</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
         <v>128</v>
@@ -2657,7 +2650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2892,13 +2885,13 @@
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B17" s="3">
         <v>2000</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
         <v>128</v>
@@ -2906,13 +2899,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="3">
         <v>2006</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>182</v>
+      <c r="C18" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="D18" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
add Smith et al., 1995 to `CBM thickness (rat)` sheet and check if `Selected` status of all included references is `Yes`
</commit_message>
<xml_diff>
--- a/data/papers/paper_list_MetaAnalysis.xlsx
+++ b/data/papers/paper_list_MetaAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2841BC58-AB3E-C642-BA42-46C653EAA050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A332F-8D60-9D41-AF61-952D17AC1EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="5" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
+    <workbookView xWindow="14700" yWindow="760" windowWidth="14700" windowHeight="16700" firstSheet="5" activeTab="7" xr2:uid="{E4C1D817-D5BA-2544-9C7F-6C83841D44D9}"/>
   </bookViews>
   <sheets>
     <sheet name="adipocyte_diameter" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="185">
   <si>
     <t>Title</t>
   </si>
@@ -593,6 +593,12 @@
   </si>
   <si>
     <t>Regional differences in the morphological and functional effects of aging on cerebral basement membranes and perivascular drainage of amyloid‐β from the mouse brain</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Insulin-dependent diabetic microangiopathy in the inner ear</t>
   </si>
 </sst>
 </file>
@@ -621,12 +627,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -641,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -662,6 +674,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,7 +1424,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1456,7 @@
       <c r="C2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1457,7 +1470,7 @@
       <c r="C3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1471,7 +1484,7 @@
       <c r="C4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1527,7 +1540,7 @@
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1541,7 +1554,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1573,7 +1586,7 @@
       <c r="C2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1587,7 +1600,7 @@
       <c r="C3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1601,7 +1614,7 @@
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1615,7 +1628,7 @@
       <c r="C5" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1629,7 +1642,7 @@
       <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1684,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC275F3-CE91-9A49-A134-C82036EB8A97}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,7 +1731,7 @@
       <c r="C2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1732,7 +1745,7 @@
       <c r="C3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1746,7 +1759,7 @@
       <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1760,7 +1773,7 @@
       <c r="C5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1774,7 +1787,7 @@
       <c r="C6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1788,7 +1801,7 @@
       <c r="C7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1802,7 +1815,7 @@
       <c r="C8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1816,7 +1829,7 @@
       <c r="C9" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1830,7 +1843,7 @@
       <c r="C10" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1841,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302E5F97-8FD7-8140-BE35-FFD37E06A9EB}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,7 +1889,7 @@
       <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1890,7 +1903,7 @@
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1904,7 +1917,7 @@
       <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1918,7 +1931,7 @@
       <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1932,7 +1945,7 @@
       <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1960,7 +1973,7 @@
       <c r="C8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2030,7 +2043,7 @@
       <c r="C13" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2072,7 +2085,7 @@
       <c r="C16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2087,7 +2100,7 @@
         <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2100,7 +2113,7 @@
       <c r="C18" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2114,7 +2127,7 @@
       <c r="C19" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2128,7 +2141,7 @@
       <c r="C20" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2142,7 +2155,7 @@
       <c r="C21" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2156,7 +2169,7 @@
       <c r="C22" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2170,7 +2183,7 @@
       <c r="C23" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2184,7 +2197,7 @@
       <c r="C24" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2198,7 +2211,7 @@
       <c r="C25" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2212,7 +2225,7 @@
       <c r="C26" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2226,7 +2239,7 @@
       <c r="C27" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2240,7 +2253,7 @@
       <c r="C28" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2254,7 +2267,7 @@
       <c r="C29" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2268,7 +2281,7 @@
       <c r="C30" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2282,7 +2295,7 @@
       <c r="C31" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2296,7 +2309,7 @@
       <c r="C32" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2310,7 +2323,7 @@
       <c r="C33" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2324,8 +2337,22 @@
       <c r="C34" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D34" t="s">
-        <v>128</v>
+      <c r="D34" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1995</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D6FC1A-79B6-5148-9205-96EE3068F7ED}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2371,7 +2398,7 @@
       <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2385,7 +2412,7 @@
       <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2413,7 +2440,7 @@
       <c r="C5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2427,7 +2454,7 @@
       <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2441,7 +2468,7 @@
       <c r="C7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2455,7 +2482,7 @@
       <c r="C8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2469,7 +2496,7 @@
       <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2483,7 +2510,7 @@
       <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2497,7 +2524,7 @@
       <c r="C11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2511,7 +2538,7 @@
       <c r="C12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2525,7 +2552,7 @@
       <c r="C13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2609,7 +2636,7 @@
       <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2623,7 +2650,7 @@
       <c r="C20" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2637,7 +2664,7 @@
       <c r="C21" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2650,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14993FC-0639-C64F-AE52-58F25C040B7B}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2683,7 +2710,7 @@
       <c r="C2" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2697,7 +2724,7 @@
       <c r="C3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2711,7 +2738,7 @@
       <c r="C4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2767,7 +2794,7 @@
       <c r="C8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2781,7 +2808,7 @@
       <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2809,7 +2836,7 @@
       <c r="C11" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2823,7 +2850,7 @@
       <c r="C12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2893,7 +2920,7 @@
       <c r="C17" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="8" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2907,7 +2934,7 @@
       <c r="C18" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="8" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>